<commit_message>
Add better version of excel
</commit_message>
<xml_diff>
--- a/Excel-Calcul_Moyenne/Calcul_Moyenne_Semestre_6.xlsx
+++ b/Excel-Calcul_Moyenne/Calcul_Moyenne_Semestre_6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romeo\Desktop\Cours\template-word-ESIREM\Excel-Calcul_Moyenne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FE2F812-2893-4E2E-9887-75A0179B7EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32012470-D6E3-4213-9D3D-9FBB7754A7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -122,7 +122,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -776,233 +776,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="13" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="13" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="13" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="9" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1012,179 +787,138 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="8" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="8" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="14" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="14" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="7" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="13" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="13" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="13" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="13" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="15" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="15" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="13" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="13" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="13" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="13" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="13" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="13" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="13" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="7" fillId="11" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1194,12 +928,278 @@
     <xf numFmtId="2" fontId="7" fillId="11" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="7" fillId="15" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="15" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="9" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="7" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="8" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="8" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="14" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="14" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1425,7 +1425,7 @@
   <dimension ref="A1:V1002"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+      <selection activeCell="J11" sqref="J11:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1434,10 +1434,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="14.25" customHeight="1">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="149" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15"/>
+      <c r="C1" s="150"/>
       <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1445,10 +1445,10 @@
         <f>B3+D3</f>
         <v>10</v>
       </c>
-      <c r="F1" s="82" t="s">
+      <c r="F1" s="141" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="9"/>
+      <c r="G1" s="142"/>
       <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1456,10 +1456,10 @@
         <f>F3+H3</f>
         <v>8</v>
       </c>
-      <c r="J1" s="83" t="s">
+      <c r="J1" s="148" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="9"/>
+      <c r="K1" s="142"/>
       <c r="L1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1467,1229 +1467,1229 @@
         <f>J3+L3</f>
         <v>6</v>
       </c>
-      <c r="N1" s="84" t="s">
+      <c r="N1" s="143" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="S1" s="10"/>
-      <c r="T1" s="12">
+      <c r="O1" s="144"/>
+      <c r="P1" s="144"/>
+      <c r="Q1" s="144"/>
+      <c r="R1" s="145" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" s="144"/>
+      <c r="T1" s="146">
         <f>N3+T3+R3+P3</f>
         <v>6</v>
       </c>
-      <c r="U1" s="13"/>
+      <c r="U1" s="147"/>
     </row>
     <row r="2" spans="1:22" ht="14.25" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="139" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="29" t="s">
+      <c r="C2" s="140"/>
+      <c r="D2" s="139" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="17" t="s">
+      <c r="E2" s="140"/>
+      <c r="F2" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19" t="s">
+      <c r="G2" s="152"/>
+      <c r="H2" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="25" t="s">
+      <c r="I2" s="121"/>
+      <c r="J2" s="154" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="26"/>
-      <c r="L2" s="27" t="s">
+      <c r="K2" s="155"/>
+      <c r="L2" s="137" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="28"/>
-      <c r="N2" s="21" t="s">
+      <c r="M2" s="138"/>
+      <c r="N2" s="122" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="22"/>
-      <c r="P2" s="21" t="s">
+      <c r="O2" s="123"/>
+      <c r="P2" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="24" t="s">
+      <c r="Q2" s="158"/>
+      <c r="R2" s="159" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="23"/>
-      <c r="T2" s="21" t="s">
+      <c r="S2" s="158"/>
+      <c r="T2" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="U2" s="23"/>
+      <c r="U2" s="158"/>
     </row>
     <row r="3" spans="1:22" ht="14.25" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="38">
+      <c r="B3" s="135">
         <v>5</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="38">
+      <c r="C3" s="136"/>
+      <c r="D3" s="135">
         <v>5</v>
       </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="31">
+      <c r="E3" s="136"/>
+      <c r="F3" s="153">
         <v>5</v>
       </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="33">
+      <c r="G3" s="125"/>
+      <c r="H3" s="124">
         <v>3</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="36">
+      <c r="I3" s="125"/>
+      <c r="J3" s="156">
         <v>4</v>
       </c>
-      <c r="K3" s="37"/>
-      <c r="L3" s="36">
+      <c r="K3" s="157"/>
+      <c r="L3" s="156">
         <v>2</v>
       </c>
-      <c r="M3" s="37"/>
-      <c r="N3" s="34">
+      <c r="M3" s="157"/>
+      <c r="N3" s="126">
         <v>1.5</v>
       </c>
-      <c r="O3" s="35"/>
-      <c r="P3" s="34">
+      <c r="O3" s="127"/>
+      <c r="P3" s="126">
         <v>1.5</v>
       </c>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="34">
+      <c r="Q3" s="127"/>
+      <c r="R3" s="126">
         <v>1</v>
       </c>
-      <c r="S3" s="35"/>
-      <c r="T3" s="34">
+      <c r="S3" s="127"/>
+      <c r="T3" s="126">
         <v>2</v>
       </c>
-      <c r="U3" s="35"/>
+      <c r="U3" s="127"/>
     </row>
     <row r="4" spans="1:22" ht="14.25" customHeight="1">
-      <c r="A4" s="16"/>
-      <c r="B4" s="44" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="106" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="44" t="s">
+      <c r="C4" s="110"/>
+      <c r="D4" s="106" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="46"/>
-      <c r="F4" s="40" t="s">
+      <c r="E4" s="107"/>
+      <c r="F4" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="41"/>
-      <c r="H4" s="40" t="s">
+      <c r="G4" s="52"/>
+      <c r="H4" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="41"/>
-      <c r="J4" s="42" t="s">
+      <c r="I4" s="52"/>
+      <c r="J4" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="43"/>
-      <c r="L4" s="42" t="s">
+      <c r="K4" s="84"/>
+      <c r="L4" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="43"/>
-      <c r="N4" s="91"/>
-      <c r="O4" s="92"/>
-      <c r="P4" s="92"/>
-      <c r="Q4" s="92"/>
-      <c r="R4" s="92"/>
-      <c r="S4" s="92"/>
-      <c r="T4" s="92"/>
-      <c r="U4" s="93"/>
+      <c r="M4" s="84"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="35"/>
+      <c r="R4" s="35"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="36"/>
     </row>
     <row r="5" spans="1:22" ht="14.25" customHeight="1">
-      <c r="A5" s="16"/>
-      <c r="B5" s="51">
+      <c r="A5" s="9"/>
+      <c r="B5" s="104">
         <v>3</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="51">
-        <v>3.5</v>
-      </c>
-      <c r="E5" s="53"/>
-      <c r="F5" s="47">
+      <c r="C5" s="111"/>
+      <c r="D5" s="104">
         <v>3</v>
       </c>
-      <c r="G5" s="48"/>
-      <c r="H5" s="47">
+      <c r="E5" s="105"/>
+      <c r="F5" s="53">
         <v>3</v>
       </c>
-      <c r="I5" s="48"/>
-      <c r="J5" s="49">
+      <c r="G5" s="54"/>
+      <c r="H5" s="53">
         <v>3</v>
       </c>
-      <c r="K5" s="50"/>
-      <c r="L5" s="49">
+      <c r="I5" s="54"/>
+      <c r="J5" s="85">
+        <v>2.5</v>
+      </c>
+      <c r="K5" s="86"/>
+      <c r="L5" s="85">
         <v>2</v>
       </c>
-      <c r="M5" s="50"/>
-      <c r="N5" s="90"/>
-      <c r="O5" s="94"/>
-      <c r="P5" s="94"/>
-      <c r="Q5" s="94"/>
-      <c r="R5" s="94"/>
-      <c r="S5" s="94"/>
-      <c r="T5" s="94"/>
-      <c r="U5" s="95"/>
+      <c r="M5" s="86"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="38"/>
+      <c r="U5" s="39"/>
     </row>
     <row r="6" spans="1:22" ht="14.25" customHeight="1">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="96" t="s">
+      <c r="B6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="96" t="s">
+      <c r="C6" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="97" t="s">
+      <c r="E6" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="97" t="s">
+      <c r="G6" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="J6" s="98" t="s">
+      <c r="I6" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="98" t="s">
-        <v>0</v>
-      </c>
-      <c r="L6" s="98" t="s">
+      <c r="K6" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="98" t="s">
-        <v>0</v>
-      </c>
-      <c r="N6" s="99" t="s">
+      <c r="M6" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="P6" s="99" t="s">
+      <c r="O6" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="P6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="Q6" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="R6" s="99" t="s">
+      <c r="Q6" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="R6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="S6" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="T6" s="99" t="s">
+      <c r="S6" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="T6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="U6" s="99" t="s">
+      <c r="U6" s="14" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="14.25" customHeight="1">
-      <c r="B7" s="100">
-        <v>0</v>
-      </c>
-      <c r="C7" s="100">
-        <v>0</v>
-      </c>
-      <c r="D7" s="100">
-        <v>0</v>
-      </c>
-      <c r="E7" s="100">
-        <v>0</v>
-      </c>
-      <c r="F7" s="101">
-        <v>0</v>
-      </c>
-      <c r="G7" s="101">
-        <v>0</v>
-      </c>
-      <c r="H7" s="101">
-        <v>0</v>
-      </c>
-      <c r="I7" s="101">
-        <v>0</v>
-      </c>
-      <c r="J7" s="102">
-        <v>0</v>
-      </c>
-      <c r="K7" s="102">
-        <v>0</v>
-      </c>
-      <c r="L7" s="102">
-        <v>0</v>
-      </c>
-      <c r="M7" s="102">
-        <v>0</v>
-      </c>
-      <c r="N7" s="165">
-        <v>0</v>
-      </c>
-      <c r="O7" s="165">
-        <v>0</v>
-      </c>
-      <c r="P7" s="165">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="165">
-        <v>0</v>
-      </c>
-      <c r="R7" s="165">
-        <v>0</v>
-      </c>
-      <c r="S7" s="165">
-        <v>0</v>
-      </c>
-      <c r="T7" s="165">
-        <v>0</v>
-      </c>
-      <c r="U7" s="165">
+      <c r="B7" s="15">
+        <v>0</v>
+      </c>
+      <c r="C7" s="15">
+        <v>0</v>
+      </c>
+      <c r="D7" s="15">
+        <v>0</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0</v>
+      </c>
+      <c r="G7" s="16">
+        <v>0</v>
+      </c>
+      <c r="H7" s="16">
+        <v>0</v>
+      </c>
+      <c r="I7" s="16">
+        <v>0</v>
+      </c>
+      <c r="J7" s="17">
+        <v>0</v>
+      </c>
+      <c r="K7" s="17">
+        <v>0</v>
+      </c>
+      <c r="L7" s="17">
+        <v>0</v>
+      </c>
+      <c r="M7" s="17">
+        <v>0</v>
+      </c>
+      <c r="N7" s="20">
+        <v>0</v>
+      </c>
+      <c r="O7" s="20">
+        <v>0</v>
+      </c>
+      <c r="P7" s="20">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="20">
+        <v>0</v>
+      </c>
+      <c r="R7" s="20">
+        <v>0</v>
+      </c>
+      <c r="S7" s="20">
+        <v>0</v>
+      </c>
+      <c r="T7" s="20">
+        <v>0</v>
+      </c>
+      <c r="U7" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="14.25" customHeight="1">
-      <c r="B8" s="100">
-        <v>0</v>
-      </c>
-      <c r="C8" s="100">
-        <v>0</v>
-      </c>
-      <c r="D8" s="100">
-        <v>0</v>
-      </c>
-      <c r="E8" s="100">
-        <v>0</v>
-      </c>
-      <c r="F8" s="101">
-        <v>0</v>
-      </c>
-      <c r="G8" s="101">
-        <v>0</v>
-      </c>
-      <c r="H8" s="101">
-        <v>0</v>
-      </c>
-      <c r="I8" s="101">
-        <v>0</v>
-      </c>
-      <c r="J8" s="102">
-        <v>0</v>
-      </c>
-      <c r="K8" s="102">
-        <v>0</v>
-      </c>
-      <c r="L8" s="102">
-        <v>0</v>
-      </c>
-      <c r="M8" s="102">
-        <v>0</v>
-      </c>
-      <c r="N8" s="99">
-        <v>0</v>
-      </c>
-      <c r="O8" s="99">
-        <v>0</v>
-      </c>
-      <c r="P8" s="99">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="99">
-        <v>0</v>
-      </c>
-      <c r="R8" s="99">
-        <v>0</v>
-      </c>
-      <c r="S8" s="99">
-        <v>0</v>
-      </c>
-      <c r="T8" s="99">
-        <v>0</v>
-      </c>
-      <c r="U8" s="99">
+      <c r="B8" s="15">
+        <v>0</v>
+      </c>
+      <c r="C8" s="15">
+        <v>0</v>
+      </c>
+      <c r="D8" s="15">
+        <v>0</v>
+      </c>
+      <c r="E8" s="15">
+        <v>0</v>
+      </c>
+      <c r="F8" s="16">
+        <v>0</v>
+      </c>
+      <c r="G8" s="16">
+        <v>0</v>
+      </c>
+      <c r="H8" s="16">
+        <v>0</v>
+      </c>
+      <c r="I8" s="16">
+        <v>0</v>
+      </c>
+      <c r="J8" s="17">
+        <v>0</v>
+      </c>
+      <c r="K8" s="17">
+        <v>0</v>
+      </c>
+      <c r="L8" s="17">
+        <v>0</v>
+      </c>
+      <c r="M8" s="17">
+        <v>0</v>
+      </c>
+      <c r="N8" s="14">
+        <v>0</v>
+      </c>
+      <c r="O8" s="14">
+        <v>0</v>
+      </c>
+      <c r="P8" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="14">
+        <v>0</v>
+      </c>
+      <c r="R8" s="14">
+        <v>0</v>
+      </c>
+      <c r="S8" s="14">
+        <v>0</v>
+      </c>
+      <c r="T8" s="14">
+        <v>0</v>
+      </c>
+      <c r="U8" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="14.25" customHeight="1">
-      <c r="B9" s="100">
-        <v>0</v>
-      </c>
-      <c r="C9" s="100">
-        <v>0</v>
-      </c>
-      <c r="D9" s="100">
-        <v>0</v>
-      </c>
-      <c r="E9" s="100">
-        <v>0</v>
-      </c>
-      <c r="F9" s="101">
-        <v>0</v>
-      </c>
-      <c r="G9" s="101">
-        <v>0</v>
-      </c>
-      <c r="H9" s="101">
-        <v>0</v>
-      </c>
-      <c r="I9" s="101">
-        <v>0</v>
-      </c>
-      <c r="J9" s="102">
-        <v>0</v>
-      </c>
-      <c r="K9" s="102">
-        <v>0</v>
-      </c>
-      <c r="L9" s="102">
-        <v>0</v>
-      </c>
-      <c r="M9" s="102">
-        <v>0</v>
-      </c>
-      <c r="N9" s="99">
-        <v>0</v>
-      </c>
-      <c r="O9" s="99">
-        <v>0</v>
-      </c>
-      <c r="P9" s="99">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="99">
-        <v>0</v>
-      </c>
-      <c r="R9" s="99">
-        <v>0</v>
-      </c>
-      <c r="S9" s="99">
-        <v>0</v>
-      </c>
-      <c r="T9" s="99">
-        <v>0</v>
-      </c>
-      <c r="U9" s="99">
+      <c r="B9" s="15">
+        <v>0</v>
+      </c>
+      <c r="C9" s="15">
+        <v>0</v>
+      </c>
+      <c r="D9" s="15">
+        <v>0</v>
+      </c>
+      <c r="E9" s="15">
+        <v>0</v>
+      </c>
+      <c r="F9" s="16">
+        <v>0</v>
+      </c>
+      <c r="G9" s="16">
+        <v>0</v>
+      </c>
+      <c r="H9" s="16">
+        <v>0</v>
+      </c>
+      <c r="I9" s="16">
+        <v>0</v>
+      </c>
+      <c r="J9" s="17">
+        <v>0</v>
+      </c>
+      <c r="K9" s="17">
+        <v>0</v>
+      </c>
+      <c r="L9" s="17">
+        <v>0</v>
+      </c>
+      <c r="M9" s="17">
+        <v>0</v>
+      </c>
+      <c r="N9" s="14">
+        <v>0</v>
+      </c>
+      <c r="O9" s="14">
+        <v>0</v>
+      </c>
+      <c r="P9" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="14">
+        <v>0</v>
+      </c>
+      <c r="R9" s="14">
+        <v>0</v>
+      </c>
+      <c r="S9" s="14">
+        <v>0</v>
+      </c>
+      <c r="T9" s="14">
+        <v>0</v>
+      </c>
+      <c r="U9" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="14.25" customHeight="1">
-      <c r="B10" s="100">
-        <v>0</v>
-      </c>
-      <c r="C10" s="100">
-        <v>0</v>
-      </c>
-      <c r="D10" s="100">
-        <v>0</v>
-      </c>
-      <c r="E10" s="100">
-        <v>0</v>
-      </c>
-      <c r="F10" s="103">
-        <v>0</v>
-      </c>
-      <c r="G10" s="103">
-        <v>0</v>
-      </c>
-      <c r="H10" s="101">
-        <v>0</v>
-      </c>
-      <c r="I10" s="101">
-        <v>0</v>
-      </c>
-      <c r="J10" s="104">
-        <v>0</v>
-      </c>
-      <c r="K10" s="104">
-        <v>0</v>
-      </c>
-      <c r="L10" s="102">
-        <v>0</v>
-      </c>
-      <c r="M10" s="102">
-        <v>0</v>
-      </c>
-      <c r="N10" s="99">
-        <v>0</v>
-      </c>
-      <c r="O10" s="99">
-        <v>0</v>
-      </c>
-      <c r="P10" s="99">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="99">
-        <v>0</v>
-      </c>
-      <c r="R10" s="99">
-        <v>0</v>
-      </c>
-      <c r="S10" s="99">
-        <v>0</v>
-      </c>
-      <c r="T10" s="99">
-        <v>0</v>
-      </c>
-      <c r="U10" s="99">
+      <c r="B10" s="15">
+        <v>0</v>
+      </c>
+      <c r="C10" s="15">
+        <v>0</v>
+      </c>
+      <c r="D10" s="15">
+        <v>0</v>
+      </c>
+      <c r="E10" s="15">
+        <v>0</v>
+      </c>
+      <c r="F10" s="18">
+        <v>0</v>
+      </c>
+      <c r="G10" s="18">
+        <v>0</v>
+      </c>
+      <c r="H10" s="16">
+        <v>0</v>
+      </c>
+      <c r="I10" s="16">
+        <v>0</v>
+      </c>
+      <c r="J10" s="19">
+        <v>0</v>
+      </c>
+      <c r="K10" s="19">
+        <v>0</v>
+      </c>
+      <c r="L10" s="17">
+        <v>0</v>
+      </c>
+      <c r="M10" s="17">
+        <v>0</v>
+      </c>
+      <c r="N10" s="14">
+        <v>0</v>
+      </c>
+      <c r="O10" s="14">
+        <v>0</v>
+      </c>
+      <c r="P10" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="14">
+        <v>0</v>
+      </c>
+      <c r="R10" s="14">
+        <v>0</v>
+      </c>
+      <c r="S10" s="14">
+        <v>0</v>
+      </c>
+      <c r="T10" s="14">
+        <v>0</v>
+      </c>
+      <c r="U10" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="14.25" customHeight="1">
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="106" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="44" t="s">
+      <c r="C11" s="107"/>
+      <c r="D11" s="106" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="46"/>
-      <c r="F11" s="40" t="s">
+      <c r="E11" s="107"/>
+      <c r="F11" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="54"/>
-      <c r="H11" s="40" t="s">
+      <c r="G11" s="55"/>
+      <c r="H11" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="54"/>
-      <c r="J11" s="42" t="s">
+      <c r="I11" s="55"/>
+      <c r="J11" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="55"/>
-      <c r="L11" s="166">
-        <v>0</v>
-      </c>
-      <c r="M11" s="166">
-        <v>0</v>
-      </c>
-      <c r="N11" s="167">
-        <v>0</v>
-      </c>
-      <c r="O11" s="167">
-        <v>0</v>
-      </c>
-      <c r="P11" s="167">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="168">
-        <v>0</v>
-      </c>
-      <c r="R11" s="167">
-        <v>0</v>
-      </c>
-      <c r="S11" s="167">
-        <v>0</v>
-      </c>
-      <c r="T11" s="167">
-        <v>0</v>
-      </c>
-      <c r="U11" s="167">
+      <c r="K11" s="87"/>
+      <c r="L11" s="21">
+        <v>0</v>
+      </c>
+      <c r="M11" s="21">
+        <v>0</v>
+      </c>
+      <c r="N11" s="22">
+        <v>0</v>
+      </c>
+      <c r="O11" s="22">
+        <v>0</v>
+      </c>
+      <c r="P11" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="23">
+        <v>0</v>
+      </c>
+      <c r="R11" s="22">
+        <v>0</v>
+      </c>
+      <c r="S11" s="22">
+        <v>0</v>
+      </c>
+      <c r="T11" s="22">
+        <v>0</v>
+      </c>
+      <c r="U11" s="22">
         <v>0</v>
       </c>
       <c r="V11" s="8"/>
     </row>
     <row r="12" spans="1:22" ht="14.25" customHeight="1">
-      <c r="B12" s="51">
+      <c r="B12" s="104">
         <v>2</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="51">
+      <c r="C12" s="105"/>
+      <c r="D12" s="104">
+        <v>2</v>
+      </c>
+      <c r="E12" s="105"/>
+      <c r="F12" s="53">
+        <v>2</v>
+      </c>
+      <c r="G12" s="56"/>
+      <c r="H12" s="53">
+        <v>2</v>
+      </c>
+      <c r="I12" s="56"/>
+      <c r="J12" s="85">
         <v>1.5</v>
       </c>
-      <c r="E12" s="53"/>
-      <c r="F12" s="47">
-        <v>2</v>
-      </c>
-      <c r="G12" s="56"/>
-      <c r="H12" s="47">
-        <v>2</v>
-      </c>
-      <c r="I12" s="56"/>
-      <c r="J12" s="49">
-        <v>2</v>
-      </c>
-      <c r="K12" s="57"/>
-      <c r="L12" s="169">
-        <v>0</v>
-      </c>
-      <c r="M12" s="166">
-        <v>0</v>
-      </c>
-      <c r="N12" s="167">
-        <v>0</v>
-      </c>
-      <c r="O12" s="167">
-        <v>0</v>
-      </c>
-      <c r="P12" s="167">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="168">
-        <v>0</v>
-      </c>
-      <c r="R12" s="167">
-        <v>0</v>
-      </c>
-      <c r="S12" s="167">
-        <v>0</v>
-      </c>
-      <c r="T12" s="167">
-        <v>0</v>
-      </c>
-      <c r="U12" s="167">
+      <c r="K12" s="88"/>
+      <c r="L12" s="24">
+        <v>0</v>
+      </c>
+      <c r="M12" s="21">
+        <v>0</v>
+      </c>
+      <c r="N12" s="22">
+        <v>0</v>
+      </c>
+      <c r="O12" s="22">
+        <v>0</v>
+      </c>
+      <c r="P12" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="23">
+        <v>0</v>
+      </c>
+      <c r="R12" s="22">
+        <v>0</v>
+      </c>
+      <c r="S12" s="22">
+        <v>0</v>
+      </c>
+      <c r="T12" s="22">
+        <v>0</v>
+      </c>
+      <c r="U12" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="14.25" customHeight="1">
-      <c r="B13" s="100">
-        <v>0</v>
-      </c>
-      <c r="C13" s="100">
-        <v>0</v>
-      </c>
-      <c r="D13" s="100">
-        <v>0</v>
-      </c>
-      <c r="E13" s="100">
-        <v>0</v>
-      </c>
-      <c r="F13" s="97">
-        <v>0</v>
-      </c>
-      <c r="G13" s="97">
-        <v>0</v>
-      </c>
-      <c r="H13" s="101">
-        <v>0</v>
-      </c>
-      <c r="I13" s="101">
-        <v>0</v>
-      </c>
-      <c r="J13" s="98">
-        <v>0</v>
-      </c>
-      <c r="K13" s="98">
-        <v>0</v>
-      </c>
-      <c r="L13" s="102">
-        <v>0</v>
-      </c>
-      <c r="M13" s="102">
-        <v>0</v>
-      </c>
-      <c r="N13" s="99">
-        <v>0</v>
-      </c>
-      <c r="O13" s="99">
-        <v>0</v>
-      </c>
-      <c r="P13" s="99">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="99">
-        <v>0</v>
-      </c>
-      <c r="R13" s="99">
-        <v>0</v>
-      </c>
-      <c r="S13" s="99">
-        <v>0</v>
-      </c>
-      <c r="T13" s="99">
-        <v>0</v>
-      </c>
-      <c r="U13" s="99">
+      <c r="B13" s="15">
+        <v>0</v>
+      </c>
+      <c r="C13" s="15">
+        <v>0</v>
+      </c>
+      <c r="D13" s="15">
+        <v>0</v>
+      </c>
+      <c r="E13" s="15">
+        <v>0</v>
+      </c>
+      <c r="F13" s="12">
+        <v>0</v>
+      </c>
+      <c r="G13" s="12">
+        <v>0</v>
+      </c>
+      <c r="H13" s="16">
+        <v>0</v>
+      </c>
+      <c r="I13" s="16">
+        <v>0</v>
+      </c>
+      <c r="J13" s="13">
+        <v>0</v>
+      </c>
+      <c r="K13" s="13">
+        <v>0</v>
+      </c>
+      <c r="L13" s="17">
+        <v>0</v>
+      </c>
+      <c r="M13" s="17">
+        <v>0</v>
+      </c>
+      <c r="N13" s="14">
+        <v>0</v>
+      </c>
+      <c r="O13" s="14">
+        <v>0</v>
+      </c>
+      <c r="P13" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="14">
+        <v>0</v>
+      </c>
+      <c r="R13" s="14">
+        <v>0</v>
+      </c>
+      <c r="S13" s="14">
+        <v>0</v>
+      </c>
+      <c r="T13" s="14">
+        <v>0</v>
+      </c>
+      <c r="U13" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="14.25" customHeight="1">
-      <c r="B14" s="100">
-        <v>0</v>
-      </c>
-      <c r="C14" s="100">
-        <v>0</v>
-      </c>
-      <c r="D14" s="100">
-        <v>0</v>
-      </c>
-      <c r="E14" s="100">
-        <v>0</v>
-      </c>
-      <c r="F14" s="101">
-        <v>0</v>
-      </c>
-      <c r="G14" s="101">
-        <v>0</v>
-      </c>
-      <c r="H14" s="101">
-        <v>0</v>
-      </c>
-      <c r="I14" s="101">
-        <v>0</v>
-      </c>
-      <c r="J14" s="102">
-        <v>0</v>
-      </c>
-      <c r="K14" s="102">
-        <v>0</v>
-      </c>
-      <c r="L14" s="102">
-        <v>0</v>
-      </c>
-      <c r="M14" s="102">
-        <v>0</v>
-      </c>
-      <c r="N14" s="99">
-        <v>0</v>
-      </c>
-      <c r="O14" s="99">
-        <v>0</v>
-      </c>
-      <c r="P14" s="173">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="99">
-        <v>0</v>
-      </c>
-      <c r="R14" s="99">
-        <v>0</v>
-      </c>
-      <c r="S14" s="99">
-        <v>0</v>
-      </c>
-      <c r="T14" s="99">
-        <v>0</v>
-      </c>
-      <c r="U14" s="99">
+      <c r="B14" s="15">
+        <v>0</v>
+      </c>
+      <c r="C14" s="15">
+        <v>0</v>
+      </c>
+      <c r="D14" s="15">
+        <v>0</v>
+      </c>
+      <c r="E14" s="15">
+        <v>0</v>
+      </c>
+      <c r="F14" s="16">
+        <v>0</v>
+      </c>
+      <c r="G14" s="16">
+        <v>0</v>
+      </c>
+      <c r="H14" s="16">
+        <v>0</v>
+      </c>
+      <c r="I14" s="16">
+        <v>0</v>
+      </c>
+      <c r="J14" s="17">
+        <v>0</v>
+      </c>
+      <c r="K14" s="17">
+        <v>0</v>
+      </c>
+      <c r="L14" s="17">
+        <v>0</v>
+      </c>
+      <c r="M14" s="17">
+        <v>0</v>
+      </c>
+      <c r="N14" s="14">
+        <v>0</v>
+      </c>
+      <c r="O14" s="14">
+        <v>0</v>
+      </c>
+      <c r="P14" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="14">
+        <v>0</v>
+      </c>
+      <c r="R14" s="14">
+        <v>0</v>
+      </c>
+      <c r="S14" s="14">
+        <v>0</v>
+      </c>
+      <c r="T14" s="14">
+        <v>0</v>
+      </c>
+      <c r="U14" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="14.25" customHeight="1">
-      <c r="B15" s="100">
-        <v>0</v>
-      </c>
-      <c r="C15" s="100">
-        <v>0</v>
-      </c>
-      <c r="D15" s="100">
-        <v>0</v>
-      </c>
-      <c r="E15" s="100">
-        <v>0</v>
-      </c>
-      <c r="F15" s="101">
-        <v>0</v>
-      </c>
-      <c r="G15" s="101">
-        <v>0</v>
-      </c>
-      <c r="H15" s="101">
-        <v>0</v>
-      </c>
-      <c r="I15" s="101">
-        <v>0</v>
-      </c>
-      <c r="J15" s="102">
-        <v>0</v>
-      </c>
-      <c r="K15" s="102">
-        <v>0</v>
-      </c>
-      <c r="L15" s="102">
-        <v>0</v>
-      </c>
-      <c r="M15" s="102">
-        <v>0</v>
-      </c>
-      <c r="N15" s="99">
-        <v>0</v>
-      </c>
-      <c r="O15" s="99">
-        <v>0</v>
-      </c>
-      <c r="P15" s="99">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="99">
-        <v>0</v>
-      </c>
-      <c r="R15" s="99">
-        <v>0</v>
-      </c>
-      <c r="S15" s="99">
-        <v>0</v>
-      </c>
-      <c r="T15" s="99">
-        <v>0</v>
-      </c>
-      <c r="U15" s="99">
+      <c r="B15" s="15">
+        <v>0</v>
+      </c>
+      <c r="C15" s="15">
+        <v>0</v>
+      </c>
+      <c r="D15" s="15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="15">
+        <v>0</v>
+      </c>
+      <c r="F15" s="16">
+        <v>0</v>
+      </c>
+      <c r="G15" s="16">
+        <v>0</v>
+      </c>
+      <c r="H15" s="16">
+        <v>0</v>
+      </c>
+      <c r="I15" s="16">
+        <v>0</v>
+      </c>
+      <c r="J15" s="17">
+        <v>0</v>
+      </c>
+      <c r="K15" s="17">
+        <v>0</v>
+      </c>
+      <c r="L15" s="17">
+        <v>0</v>
+      </c>
+      <c r="M15" s="17">
+        <v>0</v>
+      </c>
+      <c r="N15" s="14">
+        <v>0</v>
+      </c>
+      <c r="O15" s="14">
+        <v>0</v>
+      </c>
+      <c r="P15" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="14">
+        <v>0</v>
+      </c>
+      <c r="R15" s="14">
+        <v>0</v>
+      </c>
+      <c r="S15" s="14">
+        <v>0</v>
+      </c>
+      <c r="T15" s="14">
+        <v>0</v>
+      </c>
+      <c r="U15" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="14.25" customHeight="1">
-      <c r="B16" s="100">
-        <v>0</v>
-      </c>
-      <c r="C16" s="100">
-        <v>0</v>
-      </c>
-      <c r="D16" s="100">
-        <v>0</v>
-      </c>
-      <c r="E16" s="100">
-        <v>0</v>
-      </c>
-      <c r="F16" s="101">
-        <v>0</v>
-      </c>
-      <c r="G16" s="101">
-        <v>0</v>
-      </c>
-      <c r="H16" s="101">
-        <v>0</v>
-      </c>
-      <c r="I16" s="101">
-        <v>0</v>
-      </c>
-      <c r="J16" s="102">
-        <v>0</v>
-      </c>
-      <c r="K16" s="102">
-        <v>0</v>
-      </c>
-      <c r="L16" s="102">
-        <v>0</v>
-      </c>
-      <c r="M16" s="102">
-        <v>0</v>
-      </c>
-      <c r="N16" s="99">
-        <v>0</v>
-      </c>
-      <c r="O16" s="99">
-        <v>0</v>
-      </c>
-      <c r="P16" s="99">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="99">
-        <v>0</v>
-      </c>
-      <c r="R16" s="99">
-        <v>0</v>
-      </c>
-      <c r="S16" s="99">
-        <v>0</v>
-      </c>
-      <c r="T16" s="99">
-        <v>0</v>
-      </c>
-      <c r="U16" s="99">
+      <c r="B16" s="15">
+        <v>0</v>
+      </c>
+      <c r="C16" s="15">
+        <v>0</v>
+      </c>
+      <c r="D16" s="15">
+        <v>0</v>
+      </c>
+      <c r="E16" s="15">
+        <v>0</v>
+      </c>
+      <c r="F16" s="16">
+        <v>0</v>
+      </c>
+      <c r="G16" s="16">
+        <v>0</v>
+      </c>
+      <c r="H16" s="16">
+        <v>0</v>
+      </c>
+      <c r="I16" s="16">
+        <v>0</v>
+      </c>
+      <c r="J16" s="17">
+        <v>0</v>
+      </c>
+      <c r="K16" s="17">
+        <v>0</v>
+      </c>
+      <c r="L16" s="17">
+        <v>0</v>
+      </c>
+      <c r="M16" s="17">
+        <v>0</v>
+      </c>
+      <c r="N16" s="14">
+        <v>0</v>
+      </c>
+      <c r="O16" s="14">
+        <v>0</v>
+      </c>
+      <c r="P16" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="14">
+        <v>0</v>
+      </c>
+      <c r="R16" s="14">
+        <v>0</v>
+      </c>
+      <c r="S16" s="14">
+        <v>0</v>
+      </c>
+      <c r="T16" s="14">
+        <v>0</v>
+      </c>
+      <c r="U16" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B17" s="105" t="s">
+      <c r="B17" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="106"/>
-      <c r="D17" s="105" t="s">
+      <c r="C17" s="118"/>
+      <c r="D17" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="107"/>
-      <c r="F17" s="108" t="s">
+      <c r="E17" s="119"/>
+      <c r="F17" s="112" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="109"/>
-      <c r="H17" s="108" t="s">
+      <c r="G17" s="113"/>
+      <c r="H17" s="112" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="110"/>
-      <c r="J17" s="111" t="s">
+      <c r="I17" s="114"/>
+      <c r="J17" s="115" t="s">
         <v>19</v>
       </c>
-      <c r="K17" s="112"/>
-      <c r="L17" s="111" t="s">
+      <c r="K17" s="134"/>
+      <c r="L17" s="115" t="s">
         <v>19</v>
       </c>
-      <c r="M17" s="113"/>
-      <c r="N17" s="114" t="s">
+      <c r="M17" s="116"/>
+      <c r="N17" s="128" t="s">
         <v>16</v>
       </c>
-      <c r="O17" s="115"/>
-      <c r="P17" s="116" t="s">
+      <c r="O17" s="129"/>
+      <c r="P17" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="Q17" s="115"/>
-      <c r="R17" s="117" t="s">
+      <c r="Q17" s="129"/>
+      <c r="R17" s="130" t="s">
         <v>16</v>
       </c>
-      <c r="S17" s="118"/>
-      <c r="T17" s="117" t="s">
+      <c r="S17" s="132"/>
+      <c r="T17" s="130" t="s">
         <v>16</v>
       </c>
-      <c r="U17" s="119"/>
+      <c r="U17" s="131"/>
     </row>
     <row r="18" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B18" s="120" t="str">
+      <c r="B18" s="162" t="str">
         <f>IF(SUM(C7:C10)=0,"Pas de notes",((B7*C7)+(B8*C8)+(B9*C9)+(B10*C10))/(C7+C8+C9+C10))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="C18" s="121"/>
-      <c r="D18" s="120" t="str">
+      <c r="C18" s="163"/>
+      <c r="D18" s="162" t="str">
         <f>IF(SUM(E7:E10)=0,"Pas de notes",((D7*E7)+(D8*E8)+(D9*E9)+(D10*E10))/(E7+E8+E9+E10))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="E18" s="122"/>
-      <c r="F18" s="123" t="str">
+      <c r="E18" s="164"/>
+      <c r="F18" s="165" t="str">
         <f>IF(SUM(G7:G10)=0,"Pas de notes",((F7*G7)+(F8*G8)+(F9*G9)+(F10*G10))/(G7+G8+G9+G10))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="G18" s="124"/>
-      <c r="H18" s="125" t="str">
+      <c r="G18" s="166"/>
+      <c r="H18" s="167" t="str">
         <f>IF(SUM(I7:I10)=0,"Pas de notes",((H7*I7)+(H8*I8)+(H9*I9)+(H10*I10))/(I7+I8+I9+I10))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="I18" s="126"/>
-      <c r="J18" s="127" t="str">
+      <c r="I18" s="168"/>
+      <c r="J18" s="174" t="str">
         <f>IF(SUM(K7:K10)=0,"Pas de notes",((J7*K7)+(J8*K8)+(J9*K9)+(J10*K10))/(K7+K8+K9+K10))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="K18" s="128"/>
-      <c r="L18" s="129" t="str">
+      <c r="K18" s="175"/>
+      <c r="L18" s="160" t="str">
         <f>IF(SUM(M7:M10)=0,"Pas de notes",((L7*M7)+(L8*M8)+(L9*M9)+(L10*M10))/(M7+M8+M9+M10))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="M18" s="130"/>
-      <c r="N18" s="131" t="str">
+      <c r="M18" s="161"/>
+      <c r="N18" s="169" t="str">
         <f>IF(SUM(O7:O16)=0,"Pas de notes",((N7*O7)+(N8*O8)+(N9*O9)+(N10*O10)+(N11*O11)+(N12*O12)+(N13*O13)+(N14*O14)+(N15*O15)+(N16*O16))/(O7+O8+O9+O10+O11+O12+O13+O14+O15+O16))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="O18" s="132"/>
-      <c r="P18" s="133" t="str">
+      <c r="O18" s="170"/>
+      <c r="P18" s="173" t="str">
         <f>IF(SUM(Q7:Q16)=0,"Pas de notes",((P7*Q7)+(P8*Q8)+(P9*Q9)+(P10*Q10)+(P11*Q11)+(P12*Q12)+(P13*Q13)+(R14*Q14)+(P15*Q15)+(P16*Q16))/(Q7+Q8+Q9+Q10+Q11+Q12+Q13+Q14+Q15+Q16))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="Q18" s="132"/>
-      <c r="R18" s="134" t="str">
+      <c r="Q18" s="170"/>
+      <c r="R18" s="171" t="str">
         <f>IF(SUM(S7:S16)=0,"Pas de notes",((R7*S7)+(R8*S8)+(R9*S9)+(R10*S10)+(R11*S11)+(R12*S12)+(R13*S13)+(R14*S14)+(R15*S15)+(R16*S16))/(S7+S8+S9+S10+S11+S12+S13+S14+S15+S16))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="S18" s="135"/>
-      <c r="T18" s="134" t="str">
+      <c r="S18" s="172"/>
+      <c r="T18" s="171" t="str">
         <f>IF(SUM(U7:U16)=0,"Pas de notes",((T7*U7)+(T8*U8)+(T9*U9)+(T10*U10)+(T11*U11)+(T12*U12)+(T13*U13)+(T14*U14)+(T15*U15)+(T16*U16))/(U7+U8+U9+U10+U11+U12+U13+U14+U15+U16))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="U18" s="135"/>
+      <c r="U18" s="172"/>
     </row>
     <row r="19" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B19" s="136" t="s">
+      <c r="B19" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="137"/>
-      <c r="D19" s="136" t="s">
+      <c r="C19" s="109"/>
+      <c r="D19" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="137"/>
-      <c r="F19" s="138" t="s">
+      <c r="E19" s="109"/>
+      <c r="F19" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="139"/>
-      <c r="H19" s="138" t="s">
+      <c r="G19" s="58"/>
+      <c r="H19" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="I19" s="139"/>
-      <c r="J19" s="140" t="s">
+      <c r="I19" s="58"/>
+      <c r="J19" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="K19" s="141"/>
-      <c r="L19" s="140"/>
-      <c r="M19" s="141"/>
-      <c r="N19" s="142" t="s">
+      <c r="K19" s="90"/>
+      <c r="L19" s="89"/>
+      <c r="M19" s="90"/>
+      <c r="N19" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="O19" s="143"/>
-      <c r="P19" s="143"/>
-      <c r="Q19" s="144"/>
-      <c r="R19" s="142" t="s">
+      <c r="O19" s="66"/>
+      <c r="P19" s="66"/>
+      <c r="Q19" s="67"/>
+      <c r="R19" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="S19" s="143"/>
-      <c r="T19" s="143"/>
-      <c r="U19" s="144"/>
+      <c r="S19" s="66"/>
+      <c r="T19" s="66"/>
+      <c r="U19" s="67"/>
     </row>
     <row r="20" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B20" s="145" t="str">
+      <c r="B20" s="92" t="str">
         <f>IF(SUM(C13:C16)=0,"Pas de notes",(B13*C13+B14*C14+B15*C15+B16*C16)/(C13+C14+C15+C16))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="C20" s="146"/>
-      <c r="D20" s="145" t="str">
+      <c r="C20" s="93"/>
+      <c r="D20" s="92" t="str">
         <f>IF(SUM(E13:E16)=0,"Pas de notes",(D13*E13+D14*E14+D15*E15+D16*E16)/(E13+E14+E15+E16))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="E20" s="146"/>
-      <c r="F20" s="147" t="str">
+      <c r="E20" s="93"/>
+      <c r="F20" s="40" t="str">
         <f>IF(SUM(G13:G16)=0,"Pas de notes",(F13*G13+F14*G14+F15*G15+F16*G16)/(G13+G14+G15+G16))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="G20" s="148"/>
-      <c r="H20" s="147" t="str">
+      <c r="G20" s="41"/>
+      <c r="H20" s="40" t="str">
         <f>IF(SUM(I13:I16)=0,"Pas de notes",(H13*I13+H14*I14+H15*I15+H16*I16)/(I13+I14+I15+I16))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="I20" s="148"/>
-      <c r="J20" s="149" t="str">
+      <c r="I20" s="41"/>
+      <c r="J20" s="77" t="str">
         <f>IF(SUM(K13:K16)=0,"Pas de notes",(J13*K13+J14*K14+J15*K15+J16*K16)/(K13+K14+K15+K16))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="K20" s="150"/>
-      <c r="L20" s="149"/>
-      <c r="M20" s="150"/>
-      <c r="N20" s="170" t="str">
+      <c r="K20" s="78"/>
+      <c r="L20" s="77"/>
+      <c r="M20" s="78"/>
+      <c r="N20" s="68" t="str">
         <f>IF(AND(R16="Pas de notes", V16="Pas de notes"), "Pas de notes", IF(R16="Pas de notes", V16, IF(P18="Pas de notes", N18, (N18+P18)/2)))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="O20" s="171"/>
-      <c r="P20" s="171"/>
-      <c r="Q20" s="172"/>
-      <c r="R20" s="170" t="str">
+      <c r="O20" s="69"/>
+      <c r="P20" s="69"/>
+      <c r="Q20" s="70"/>
+      <c r="R20" s="68" t="str">
         <f>IF(AND(V16="Pas de notes", Z16="Pas de notes"), "Pas de notes", IF(V16="Pas de notes", Z16, IF(T18="Pas de notes", R18, (R18+T18)/2)))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="S20" s="171"/>
-      <c r="T20" s="171"/>
-      <c r="U20" s="172"/>
+      <c r="S20" s="69"/>
+      <c r="T20" s="69"/>
+      <c r="U20" s="70"/>
     </row>
     <row r="21" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B21" s="151" t="s">
+      <c r="B21" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="152"/>
-      <c r="D21" s="151" t="s">
+      <c r="C21" s="95"/>
+      <c r="D21" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="152"/>
-      <c r="F21" s="153" t="s">
+      <c r="E21" s="95"/>
+      <c r="F21" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="154"/>
-      <c r="H21" s="153" t="s">
+      <c r="G21" s="43"/>
+      <c r="H21" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="I21" s="155"/>
-      <c r="J21" s="156" t="s">
+      <c r="I21" s="59"/>
+      <c r="J21" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="K21" s="157"/>
-      <c r="L21" s="158" t="s">
+      <c r="K21" s="80"/>
+      <c r="L21" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="M21" s="157"/>
-      <c r="N21" s="76" t="s">
+      <c r="M21" s="80"/>
+      <c r="N21" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="O21" s="77"/>
-      <c r="P21" s="77"/>
-      <c r="Q21" s="77"/>
-      <c r="R21" s="77"/>
-      <c r="S21" s="77"/>
-      <c r="T21" s="77"/>
-      <c r="U21" s="78"/>
+      <c r="O21" s="72"/>
+      <c r="P21" s="72"/>
+      <c r="Q21" s="72"/>
+      <c r="R21" s="72"/>
+      <c r="S21" s="72"/>
+      <c r="T21" s="72"/>
+      <c r="U21" s="73"/>
     </row>
     <row r="22" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B22" s="159" t="str">
+      <c r="B22" s="96" t="str">
         <f>IF(AND(B18="Pas de notes", B20="Pas de notes"), "Pas de notes", IF(B18="Pas de notes", B20, IF(B20="Pas de notes", B18, (B18*B5+B20*B12)/(B12+B5))))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="C22" s="160"/>
-      <c r="D22" s="159" t="str">
+      <c r="C22" s="97"/>
+      <c r="D22" s="96" t="str">
         <f>IF(AND(D18="Pas de notes", D20="Pas de notes"), "Pas de notes", IF(D18="Pas de notes", D20, IF(D20="Pas de notes", D18, (D18*D5+D20*D12)/(D12+D5))))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="E22" s="160"/>
-      <c r="F22" s="161" t="str">
+      <c r="E22" s="97"/>
+      <c r="F22" s="44" t="str">
         <f>IF(AND(F18="Pas de notes", F20="Pas de notes"), "Pas de notes", IF(F18="Pas de notes", F20, IF(F20="Pas de notes", F18, (F18*F5+F20*F12)/(F12+F5))))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="G22" s="162"/>
-      <c r="H22" s="161" t="str">
+      <c r="G22" s="45"/>
+      <c r="H22" s="44" t="str">
         <f>IF(AND(H18="Pas de notes", H20="Pas de notes"), "Pas de notes", IF(H18="Pas de notes", H20, IF(H20="Pas de notes", H18, (H18*H5+H20*H12)/(H12+H5))))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="I22" s="162"/>
-      <c r="J22" s="163" t="str">
+      <c r="I22" s="45"/>
+      <c r="J22" s="81" t="str">
         <f>IF(AND(J18="Pas de notes", J20="Pas de notes"), "Pas de notes", IF(J18="Pas de notes", J20, IF(J20="Pas de notes", J18, (J18*J5+J20*J12)/(J12+J5))))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="K22" s="164"/>
-      <c r="L22" s="163" t="str">
+      <c r="K22" s="82"/>
+      <c r="L22" s="81" t="str">
         <f>IF(OR(L18="Pas de notes", L20="Pas de notes"),"Pas de notes",((L18*L5+L20*L12)/(L12+L5)))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="M22" s="164"/>
-      <c r="N22" s="79"/>
-      <c r="O22" s="80"/>
-      <c r="P22" s="80"/>
-      <c r="Q22" s="80"/>
-      <c r="R22" s="80"/>
-      <c r="S22" s="80"/>
-      <c r="T22" s="80"/>
-      <c r="U22" s="81"/>
+      <c r="M22" s="82"/>
+      <c r="N22" s="74"/>
+      <c r="O22" s="75"/>
+      <c r="P22" s="75"/>
+      <c r="Q22" s="75"/>
+      <c r="R22" s="75"/>
+      <c r="S22" s="75"/>
+      <c r="T22" s="75"/>
+      <c r="U22" s="76"/>
     </row>
     <row r="23" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B23" s="60" t="s">
+      <c r="B23" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="58" t="s">
+      <c r="C23" s="99"/>
+      <c r="D23" s="99"/>
+      <c r="E23" s="100"/>
+      <c r="F23" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="69" t="s">
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="K23" s="69"/>
-      <c r="L23" s="69"/>
-      <c r="M23" s="59"/>
-      <c r="N23" s="79"/>
-      <c r="O23" s="80"/>
-      <c r="P23" s="80"/>
-      <c r="Q23" s="80"/>
-      <c r="R23" s="80"/>
-      <c r="S23" s="80"/>
-      <c r="T23" s="80"/>
-      <c r="U23" s="81"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="60"/>
+      <c r="M23" s="61"/>
+      <c r="N23" s="74"/>
+      <c r="O23" s="75"/>
+      <c r="P23" s="75"/>
+      <c r="Q23" s="75"/>
+      <c r="R23" s="75"/>
+      <c r="S23" s="75"/>
+      <c r="T23" s="75"/>
+      <c r="U23" s="76"/>
     </row>
     <row r="24" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B24" s="66" t="str">
+      <c r="B24" s="101" t="str">
         <f>IF(AND(B22="Pas de notes", D22="Pas de notes"), "Pas de notes", IF(B22="Pas de notes", D22, IF(D22="Pas de notes", B22, (B22+D22)/2)))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="62" t="str">
+      <c r="C24" s="102"/>
+      <c r="D24" s="102"/>
+      <c r="E24" s="103"/>
+      <c r="F24" s="48" t="str">
         <f>IF(AND(F22="Pas de notes", H22="Pas de notes"), "Pas de notes", IF(F22="Pas de notes", H22, IF(H22="Pas de notes", F22, (F22+H22)/2)))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="G24" s="70"/>
-      <c r="H24" s="70"/>
-      <c r="I24" s="63"/>
-      <c r="J24" s="64" t="str">
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="62" t="str">
         <f>IF(AND(N20="Pas de notes", R20="Pas de notes"), "Pas de notes", IF(N20="Pas de notes", R20, IF(L22="Pas de notes", J22, (J22+L22)/2)))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="K24" s="71"/>
-      <c r="L24" s="71"/>
-      <c r="M24" s="65"/>
-      <c r="N24" s="170" t="str">
+      <c r="K24" s="63"/>
+      <c r="L24" s="63"/>
+      <c r="M24" s="64"/>
+      <c r="N24" s="68" t="str">
         <f>IF(AND(R16="Pas de notes", V16="Pas de notes"), "Pas de notes", IF(R16="Pas de notes", V16, IF(P18="Pas de notes", N18, (N18+P18)/2)))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="O24" s="171"/>
-      <c r="P24" s="171"/>
-      <c r="Q24" s="171"/>
-      <c r="R24" s="171"/>
-      <c r="S24" s="171"/>
-      <c r="T24" s="171"/>
-      <c r="U24" s="172"/>
+      <c r="O24" s="69"/>
+      <c r="P24" s="69"/>
+      <c r="Q24" s="69"/>
+      <c r="R24" s="69"/>
+      <c r="S24" s="69"/>
+      <c r="T24" s="69"/>
+      <c r="U24" s="70"/>
     </row>
     <row r="25" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B25" s="85" t="s">
+      <c r="B25" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="74"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="74"/>
-      <c r="H25" s="74"/>
-      <c r="I25" s="74"/>
-      <c r="J25" s="74"/>
-      <c r="K25" s="74"/>
-      <c r="L25" s="74"/>
-      <c r="M25" s="74"/>
-      <c r="N25" s="74"/>
-      <c r="O25" s="74"/>
-      <c r="P25" s="74"/>
-      <c r="Q25" s="74"/>
-      <c r="R25" s="74"/>
-      <c r="S25" s="74"/>
-      <c r="T25" s="74"/>
-      <c r="U25" s="86"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="27"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="27"/>
+      <c r="Q25" s="27"/>
+      <c r="R25" s="27"/>
+      <c r="S25" s="27"/>
+      <c r="T25" s="27"/>
+      <c r="U25" s="28"/>
     </row>
     <row r="26" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B26" s="87"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="75"/>
-      <c r="H26" s="75"/>
-      <c r="I26" s="75"/>
-      <c r="J26" s="75"/>
-      <c r="K26" s="75"/>
-      <c r="L26" s="75"/>
-      <c r="M26" s="75"/>
-      <c r="N26" s="75"/>
-      <c r="O26" s="75"/>
-      <c r="P26" s="75"/>
-      <c r="Q26" s="75"/>
-      <c r="R26" s="75"/>
-      <c r="S26" s="75"/>
-      <c r="T26" s="75"/>
-      <c r="U26" s="88"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="30"/>
+      <c r="R26" s="30"/>
+      <c r="S26" s="30"/>
+      <c r="T26" s="30"/>
+      <c r="U26" s="31"/>
     </row>
     <row r="27" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B27" s="89"/>
-      <c r="C27" s="174" t="str">
+      <c r="B27" s="10"/>
+      <c r="C27" s="32" t="str">
         <f>IF(AND(B24="Pas de notes", F24="Pas de notes", N24="Pas de notes", J24="Pas de notes"), "Pas de notes", (IF(B24="Pas de notes", 0, B24*(B3+D3)) + IF(F24="Pas de notes", 0, F24*(F3+H3)) + IF(N24="Pas de notes", 0, N24*(N3+P3+R3+T3)) + IF(J24="Pas de notes", 0, J24*(J3+L3))) / (IF(B24="Pas de notes", 0, B3+D3) + IF(F24="Pas de notes", 0, F3+H3) + IF(N24="Pas de notes", 0, N3+P3+R3+T3) + IF(J24="Pas de notes", 0, J3+L3)))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="D27" s="174"/>
-      <c r="E27" s="174"/>
-      <c r="F27" s="174"/>
-      <c r="G27" s="174"/>
-      <c r="H27" s="174"/>
-      <c r="I27" s="174"/>
-      <c r="J27" s="174"/>
-      <c r="K27" s="174"/>
-      <c r="L27" s="174"/>
-      <c r="M27" s="174"/>
-      <c r="N27" s="174"/>
-      <c r="O27" s="174"/>
-      <c r="P27" s="174"/>
-      <c r="Q27" s="174"/>
-      <c r="R27" s="174"/>
-      <c r="S27" s="174"/>
-      <c r="T27" s="174"/>
-      <c r="U27" s="175"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="32"/>
+      <c r="Q27" s="32"/>
+      <c r="R27" s="32"/>
+      <c r="S27" s="32"/>
+      <c r="T27" s="32"/>
+      <c r="U27" s="33"/>
     </row>
     <row r="28" spans="2:21" ht="14.25" customHeight="1"/>
     <row r="29" spans="2:21" ht="14.25" customHeight="1"/>
@@ -3668,6 +3668,89 @@
     <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="107">
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L19:M19"/>
     <mergeCell ref="B25:U26"/>
     <mergeCell ref="C27:U27"/>
     <mergeCell ref="N4:U5"/>
@@ -3692,89 +3775,6 @@
     <mergeCell ref="R20:U20"/>
     <mergeCell ref="N21:U23"/>
     <mergeCell ref="N24:U24"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="J18:K18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
fix calcul moyenne issues
</commit_message>
<xml_diff>
--- a/Excel-Calcul_Moyenne/Calcul_Moyenne_Semestre_6.xlsx
+++ b/Excel-Calcul_Moyenne/Calcul_Moyenne_Semestre_6.xlsx
@@ -1,22 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romeo\Desktop\Cours\template-word-ESIREM\Excel-Calcul_Moyenne\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugog\OneDrive\Bureau\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{651C7B59-3F6F-45D9-966D-8F1FB1836270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD82BDE-D6D6-48F9-BFCD-285C815EEEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="mb/LMxdLbD3uUYz3v/zqk8v1EVmF2wsw+J5wjnKXpwA="/>
     </ext>
@@ -758,7 +769,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -791,31 +802,370 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="15" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="15" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="13" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="13" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="13" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="13" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="13" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="13" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="13" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="11" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="11" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="9" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="8" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="7" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="8" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="7" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="8" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="8" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -853,353 +1203,13 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="9" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="15" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="15" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="13" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="13" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="13" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="13" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="13" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="13" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="13" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="11" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="11" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1424,20 +1434,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="21" width="11.44140625" customWidth="1"/>
+    <col min="1" max="21" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="14.25" customHeight="1">
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="139" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="68"/>
+      <c r="C1" s="140"/>
       <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1445,10 +1455,10 @@
         <f>B3+D3</f>
         <v>10</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="131" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="60"/>
+      <c r="G1" s="132"/>
       <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1456,10 +1466,10 @@
         <f>F3+H3</f>
         <v>8</v>
       </c>
-      <c r="J1" s="66" t="s">
+      <c r="J1" s="138" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="60"/>
+      <c r="K1" s="132"/>
       <c r="L1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1467,181 +1477,181 @@
         <f>J3+L3</f>
         <v>6</v>
       </c>
-      <c r="N1" s="61" t="s">
+      <c r="N1" s="133" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="S1" s="62"/>
-      <c r="T1" s="64">
+      <c r="O1" s="134"/>
+      <c r="P1" s="134"/>
+      <c r="Q1" s="134"/>
+      <c r="R1" s="135" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" s="134"/>
+      <c r="T1" s="136">
         <f>N3+T3+R3+P3</f>
         <v>6</v>
       </c>
-      <c r="U1" s="65"/>
+      <c r="U1" s="137"/>
     </row>
     <row r="2" spans="1:22" ht="14.25" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="154" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="57" t="s">
+      <c r="C2" s="155"/>
+      <c r="D2" s="154" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="58"/>
-      <c r="F2" s="69" t="s">
+      <c r="E2" s="155"/>
+      <c r="F2" s="141" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="70"/>
-      <c r="H2" s="87" t="s">
+      <c r="G2" s="142"/>
+      <c r="H2" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="88"/>
-      <c r="J2" s="73" t="s">
+      <c r="I2" s="113"/>
+      <c r="J2" s="144" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="74"/>
-      <c r="L2" s="55" t="s">
+      <c r="K2" s="145"/>
+      <c r="L2" s="152" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="56"/>
-      <c r="N2" s="28" t="s">
+      <c r="M2" s="153"/>
+      <c r="N2" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="89"/>
-      <c r="P2" s="28" t="s">
+      <c r="O2" s="115"/>
+      <c r="P2" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="77" t="s">
+      <c r="Q2" s="150"/>
+      <c r="R2" s="151" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="29"/>
-      <c r="T2" s="28" t="s">
+      <c r="S2" s="150"/>
+      <c r="T2" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="U2" s="29"/>
+      <c r="U2" s="150"/>
     </row>
     <row r="3" spans="1:22" ht="14.25" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="53">
+      <c r="B3" s="148">
         <v>5</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="53">
+      <c r="C3" s="149"/>
+      <c r="D3" s="148">
         <v>5</v>
       </c>
-      <c r="E3" s="54"/>
-      <c r="F3" s="71">
+      <c r="E3" s="149"/>
+      <c r="F3" s="143">
         <v>5</v>
       </c>
-      <c r="G3" s="72"/>
-      <c r="H3" s="90">
+      <c r="G3" s="117"/>
+      <c r="H3" s="116">
         <v>3</v>
       </c>
-      <c r="I3" s="72"/>
-      <c r="J3" s="75">
+      <c r="I3" s="117"/>
+      <c r="J3" s="146">
         <v>4</v>
       </c>
-      <c r="K3" s="76"/>
-      <c r="L3" s="75">
+      <c r="K3" s="147"/>
+      <c r="L3" s="146">
         <v>2</v>
       </c>
-      <c r="M3" s="76"/>
-      <c r="N3" s="26">
+      <c r="M3" s="147"/>
+      <c r="N3" s="118">
         <v>1.5</v>
       </c>
-      <c r="O3" s="27"/>
-      <c r="P3" s="26">
+      <c r="O3" s="119"/>
+      <c r="P3" s="118">
         <v>1.5</v>
       </c>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="26">
+      <c r="Q3" s="119"/>
+      <c r="R3" s="118">
         <v>1</v>
       </c>
-      <c r="S3" s="27"/>
-      <c r="T3" s="26">
+      <c r="S3" s="119"/>
+      <c r="T3" s="118">
         <v>2</v>
       </c>
-      <c r="U3" s="27"/>
+      <c r="U3" s="119"/>
     </row>
     <row r="4" spans="1:22" ht="14.25" customHeight="1">
       <c r="A4" s="9"/>
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="104"/>
-      <c r="D4" s="98" t="s">
+      <c r="C4" s="126"/>
+      <c r="D4" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="99"/>
-      <c r="F4" s="91" t="s">
+      <c r="E4" s="123"/>
+      <c r="F4" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="92"/>
-      <c r="H4" s="91" t="s">
+      <c r="G4" s="51"/>
+      <c r="H4" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="92"/>
-      <c r="J4" s="124" t="s">
+      <c r="I4" s="51"/>
+      <c r="J4" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="125"/>
-      <c r="L4" s="124" t="s">
+      <c r="K4" s="83"/>
+      <c r="L4" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="125"/>
-      <c r="N4" s="141"/>
-      <c r="O4" s="142"/>
-      <c r="P4" s="142"/>
-      <c r="Q4" s="142"/>
-      <c r="R4" s="142"/>
-      <c r="S4" s="142"/>
-      <c r="T4" s="142"/>
-      <c r="U4" s="143"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="34"/>
+      <c r="U4" s="35"/>
     </row>
     <row r="5" spans="1:22" ht="14.25" customHeight="1">
       <c r="A5" s="9"/>
-      <c r="B5" s="100">
+      <c r="B5" s="103">
         <v>3</v>
       </c>
-      <c r="C5" s="105"/>
-      <c r="D5" s="100">
-        <v>3.5</v>
-      </c>
-      <c r="E5" s="101"/>
-      <c r="F5" s="93">
+      <c r="C5" s="127"/>
+      <c r="D5" s="103">
         <v>3</v>
       </c>
-      <c r="G5" s="94"/>
-      <c r="H5" s="93">
+      <c r="E5" s="104"/>
+      <c r="F5" s="52">
         <v>3</v>
       </c>
-      <c r="I5" s="94"/>
-      <c r="J5" s="126">
+      <c r="G5" s="53"/>
+      <c r="H5" s="52">
         <v>3</v>
       </c>
-      <c r="K5" s="127"/>
-      <c r="L5" s="126">
+      <c r="I5" s="53"/>
+      <c r="J5" s="84">
+        <v>2.5</v>
+      </c>
+      <c r="K5" s="85"/>
+      <c r="L5" s="84">
         <v>2</v>
       </c>
-      <c r="M5" s="127"/>
-      <c r="N5" s="144"/>
-      <c r="O5" s="145"/>
-      <c r="P5" s="145"/>
-      <c r="Q5" s="145"/>
-      <c r="R5" s="145"/>
-      <c r="S5" s="145"/>
-      <c r="T5" s="145"/>
-      <c r="U5" s="146"/>
+      <c r="M5" s="85"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="38"/>
     </row>
     <row r="6" spans="1:22" ht="14.25" customHeight="1">
       <c r="A6" s="7" t="s">
@@ -1957,30 +1967,30 @@
       </c>
     </row>
     <row r="11" spans="1:22" ht="14.25" customHeight="1">
-      <c r="B11" s="98" t="s">
+      <c r="B11" s="122" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="99"/>
-      <c r="D11" s="98" t="s">
+      <c r="C11" s="123"/>
+      <c r="D11" s="122" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="99"/>
-      <c r="F11" s="91" t="s">
+      <c r="E11" s="123"/>
+      <c r="F11" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="95"/>
-      <c r="H11" s="91" t="s">
+      <c r="G11" s="54"/>
+      <c r="H11" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="95"/>
-      <c r="J11" s="124" t="s">
+      <c r="I11" s="54"/>
+      <c r="J11" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="128"/>
-      <c r="L11" s="21">
-        <v>0</v>
-      </c>
-      <c r="M11" s="21">
+      <c r="K11" s="86"/>
+      <c r="L11" s="17">
+        <v>0</v>
+      </c>
+      <c r="M11" s="17">
         <v>0</v>
       </c>
       <c r="N11" s="22">
@@ -2010,27 +2020,27 @@
       <c r="V11" s="8"/>
     </row>
     <row r="12" spans="1:22" ht="14.25" customHeight="1">
-      <c r="B12" s="100">
+      <c r="B12" s="103">
         <v>2</v>
       </c>
-      <c r="C12" s="101"/>
-      <c r="D12" s="100">
+      <c r="C12" s="104"/>
+      <c r="D12" s="103">
+        <v>2</v>
+      </c>
+      <c r="E12" s="104"/>
+      <c r="F12" s="52">
+        <v>2</v>
+      </c>
+      <c r="G12" s="55"/>
+      <c r="H12" s="52">
+        <v>2</v>
+      </c>
+      <c r="I12" s="55"/>
+      <c r="J12" s="84">
         <v>1.5</v>
       </c>
-      <c r="E12" s="101"/>
-      <c r="F12" s="93">
-        <v>2</v>
-      </c>
-      <c r="G12" s="96"/>
-      <c r="H12" s="93">
-        <v>2</v>
-      </c>
-      <c r="I12" s="96"/>
-      <c r="J12" s="126">
-        <v>2</v>
-      </c>
-      <c r="K12" s="129"/>
-      <c r="L12" s="24">
+      <c r="K12" s="87"/>
+      <c r="L12" s="17">
         <v>0</v>
       </c>
       <c r="M12" s="21">
@@ -2166,7 +2176,7 @@
       <c r="O14" s="14">
         <v>0</v>
       </c>
-      <c r="P14" s="25">
+      <c r="P14" s="24">
         <v>0</v>
       </c>
       <c r="Q14" s="14">
@@ -2310,386 +2320,386 @@
       </c>
     </row>
     <row r="17" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B17" s="84" t="s">
+      <c r="B17" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="85"/>
-      <c r="D17" s="84" t="s">
+      <c r="C17" s="110"/>
+      <c r="D17" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="86"/>
-      <c r="F17" s="78" t="s">
+      <c r="E17" s="111"/>
+      <c r="F17" s="172" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="79"/>
-      <c r="H17" s="78" t="s">
+      <c r="G17" s="173"/>
+      <c r="H17" s="172" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="80"/>
-      <c r="J17" s="51" t="s">
+      <c r="I17" s="174"/>
+      <c r="J17" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="K17" s="52"/>
-      <c r="L17" s="51" t="s">
+      <c r="K17" s="171"/>
+      <c r="L17" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="M17" s="83"/>
-      <c r="N17" s="97" t="s">
+      <c r="M17" s="108"/>
+      <c r="N17" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="O17" s="50"/>
-      <c r="P17" s="49" t="s">
+      <c r="O17" s="121"/>
+      <c r="P17" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="Q17" s="50"/>
-      <c r="R17" s="46" t="s">
+      <c r="Q17" s="121"/>
+      <c r="R17" s="167" t="s">
         <v>16</v>
       </c>
-      <c r="S17" s="48"/>
-      <c r="T17" s="46" t="s">
+      <c r="S17" s="169"/>
+      <c r="T17" s="167" t="s">
         <v>16</v>
       </c>
-      <c r="U17" s="47"/>
+      <c r="U17" s="168"/>
     </row>
     <row r="18" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B18" s="32" t="str">
+      <c r="B18" s="105" t="str">
         <f>IF(SUM(C7:C10)=0,"Pas de notes",((B7*C7)+(B8*C8)+(B9*C9)+(B10*C10))/(C7+C8+C9+C10))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="32" t="str">
+      <c r="C18" s="130"/>
+      <c r="D18" s="105" t="str">
         <f>IF(SUM(E7:E10)=0,"Pas de notes",((D7*E7)+(D8*E8)+(D9*E9)+(D10*E10))/(E7+E8+E9+E10))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="E18" s="34"/>
-      <c r="F18" s="35" t="str">
+      <c r="E18" s="106"/>
+      <c r="F18" s="156" t="str">
         <f>IF(SUM(G7:G10)=0,"Pas de notes",((F7*G7)+(F8*G8)+(F9*G9)+(F10*G10))/(G7+G8+G9+G10))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37" t="str">
+      <c r="G18" s="157"/>
+      <c r="H18" s="158" t="str">
         <f>IF(SUM(I7:I10)=0,"Pas de notes",((H7*I7)+(H8*I8)+(H9*I9)+(H10*I10))/(I7+I8+I9+I10))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="I18" s="38"/>
-      <c r="J18" s="44" t="str">
+      <c r="I18" s="159"/>
+      <c r="J18" s="165" t="str">
         <f>IF(SUM(K7:K10)=0,"Pas de notes",((J7*K7)+(J8*K8)+(J9*K9)+(J10*K10))/(K7+K8+K9+K10))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="K18" s="45"/>
-      <c r="L18" s="30" t="str">
+      <c r="K18" s="166"/>
+      <c r="L18" s="128" t="str">
         <f>IF(SUM(M7:M10)=0,"Pas de notes",((L7*M7)+(L8*M8)+(L9*M9)+(L10*M10))/(M7+M8+M9+M10))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="M18" s="31"/>
-      <c r="N18" s="39" t="str">
+      <c r="M18" s="129"/>
+      <c r="N18" s="160" t="str">
         <f>IF(SUM(O7:O16)=0,"Pas de notes",((N7*O7)+(N8*O8)+(N9*O9)+(N10*O10)+(N11*O11)+(N12*O12)+(N13*O13)+(N14*O14)+(N15*O15)+(N16*O16))/(O7+O8+O9+O10+O11+O12+O13+O14+O15+O16))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="O18" s="40"/>
-      <c r="P18" s="43" t="str">
+      <c r="O18" s="161"/>
+      <c r="P18" s="164" t="str">
         <f>IF(SUM(Q7:Q16)=0,"Pas de notes",((P7*Q7)+(P8*Q8)+(P9*Q9)+(P10*Q10)+(P11*Q11)+(P12*Q12)+(P13*Q13)+(R14*Q14)+(P15*Q15)+(P16*Q16))/(Q7+Q8+Q9+Q10+Q11+Q12+Q13+Q14+Q15+Q16))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="Q18" s="40"/>
-      <c r="R18" s="41" t="str">
+      <c r="Q18" s="161"/>
+      <c r="R18" s="162" t="str">
         <f>IF(SUM(S7:S16)=0,"Pas de notes",((R7*S7)+(R8*S8)+(R9*S9)+(R10*S10)+(R11*S11)+(R12*S12)+(R13*S13)+(R14*S14)+(R15*S15)+(R16*S16))/(S7+S8+S9+S10+S11+S12+S13+S14+S15+S16))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="S18" s="42"/>
-      <c r="T18" s="41" t="str">
+      <c r="S18" s="163"/>
+      <c r="T18" s="162" t="str">
         <f>IF(SUM(U7:U16)=0,"Pas de notes",((T7*U7)+(T8*U8)+(T9*U9)+(T10*U10)+(T11*U11)+(T12*U12)+(T13*U13)+(T14*U14)+(T15*U15)+(T16*U16))/(U7+U8+U9+U10+U11+U12+U13+U14+U15+U16))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="U18" s="42"/>
+      <c r="U18" s="163"/>
     </row>
     <row r="19" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B19" s="102" t="s">
+      <c r="B19" s="124" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="103"/>
-      <c r="D19" s="102" t="s">
+      <c r="C19" s="125"/>
+      <c r="D19" s="124" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="103"/>
-      <c r="F19" s="81" t="s">
+      <c r="E19" s="125"/>
+      <c r="F19" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="82"/>
-      <c r="H19" s="81" t="s">
+      <c r="G19" s="57"/>
+      <c r="H19" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="I19" s="82"/>
-      <c r="J19" s="130" t="s">
+      <c r="I19" s="57"/>
+      <c r="J19" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="K19" s="131"/>
-      <c r="L19" s="130"/>
-      <c r="M19" s="131"/>
-      <c r="N19" s="164" t="s">
+      <c r="K19" s="89"/>
+      <c r="L19" s="88"/>
+      <c r="M19" s="89"/>
+      <c r="N19" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="O19" s="165"/>
-      <c r="P19" s="165"/>
-      <c r="Q19" s="166"/>
-      <c r="R19" s="164" t="s">
+      <c r="O19" s="65"/>
+      <c r="P19" s="65"/>
+      <c r="Q19" s="66"/>
+      <c r="R19" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="S19" s="165"/>
-      <c r="T19" s="165"/>
-      <c r="U19" s="166"/>
+      <c r="S19" s="65"/>
+      <c r="T19" s="65"/>
+      <c r="U19" s="66"/>
     </row>
     <row r="20" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B20" s="106" t="str">
+      <c r="B20" s="91" t="str">
         <f>IF(SUM(C13:C16)=0,"Pas de notes",(B13*C13+B14*C14+B15*C15+B16*C16)/(C13+C14+C15+C16))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="C20" s="107"/>
-      <c r="D20" s="106" t="str">
+      <c r="C20" s="92"/>
+      <c r="D20" s="91" t="str">
         <f>IF(SUM(E13:E16)=0,"Pas de notes",(D13*E13+D14*E14+D15*E15+D16*E16)/(E13+E14+E15+E16))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="E20" s="107"/>
-      <c r="F20" s="147" t="str">
+      <c r="E20" s="92"/>
+      <c r="F20" s="39" t="str">
         <f>IF(SUM(G13:G16)=0,"Pas de notes",(F13*G13+F14*G14+F15*G15+F16*G16)/(G13+G14+G15+G16))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="G20" s="148"/>
-      <c r="H20" s="147" t="str">
+      <c r="G20" s="40"/>
+      <c r="H20" s="39" t="str">
         <f>IF(SUM(I13:I16)=0,"Pas de notes",(H13*I13+H14*I14+H15*I15+H16*I16)/(I13+I14+I15+I16))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="I20" s="148"/>
-      <c r="J20" s="118" t="str">
+      <c r="I20" s="40"/>
+      <c r="J20" s="76" t="str">
         <f>IF(SUM(K13:K16)=0,"Pas de notes",(J13*K13+J14*K14+J15*K15+J16*K16)/(K13+K14+K15+K16))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="K20" s="119"/>
-      <c r="L20" s="118"/>
-      <c r="M20" s="119"/>
-      <c r="N20" s="167" t="str">
-        <f>IF(AND(N18="Pas de notes", P18="Pas de notes"), "Pas de notes", IF(N18="Pas de notes", P18, IF(P18="Pas de notes", N18, (N18+P18)/2)))</f>
+      <c r="K20" s="77"/>
+      <c r="L20" s="76"/>
+      <c r="M20" s="77"/>
+      <c r="N20" s="67" t="str">
+        <f>IF(AND(N18="Pas de notes",P18="Pas de notes"),"Pas de notes",IF(N18="Pas de notes",P18,IF(P18="Pas de notes",N18,(N18*N3+P18*P3)/(N3+P3))))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="O20" s="168"/>
-      <c r="P20" s="168"/>
-      <c r="Q20" s="169"/>
-      <c r="R20" s="167" t="str">
-        <f>IF(AND(R18="Pas de notes", T18="Pas de notes"), "Pas de notes", IF(R18="Pas de notes", T18, IF(T18="Pas de notes", R18, (R18+T18)/2)))</f>
+      <c r="O20" s="68"/>
+      <c r="P20" s="68"/>
+      <c r="Q20" s="69"/>
+      <c r="R20" s="67" t="str">
+        <f>IF(AND(R18="Pas de notes",T18="Pas de notes"),"Pas de notes",IF(R18="Pas de notes",T18,IF(T18="Pas de notes",R18,(R18*R3+T18*T3)/(R3+T3))))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="S20" s="168"/>
-      <c r="T20" s="168"/>
-      <c r="U20" s="169"/>
+      <c r="S20" s="68"/>
+      <c r="T20" s="68"/>
+      <c r="U20" s="69"/>
     </row>
     <row r="21" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B21" s="108" t="s">
+      <c r="B21" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="109"/>
-      <c r="D21" s="108" t="s">
+      <c r="C21" s="94"/>
+      <c r="D21" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="109"/>
-      <c r="F21" s="149" t="s">
+      <c r="E21" s="94"/>
+      <c r="F21" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="150"/>
-      <c r="H21" s="149" t="s">
+      <c r="G21" s="42"/>
+      <c r="H21" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="I21" s="158"/>
-      <c r="J21" s="132" t="s">
+      <c r="I21" s="58"/>
+      <c r="J21" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="K21" s="121"/>
-      <c r="L21" s="120" t="s">
+      <c r="K21" s="79"/>
+      <c r="L21" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="M21" s="121"/>
-      <c r="N21" s="170" t="s">
+      <c r="M21" s="79"/>
+      <c r="N21" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="O21" s="171"/>
-      <c r="P21" s="171"/>
-      <c r="Q21" s="171"/>
-      <c r="R21" s="171"/>
-      <c r="S21" s="171"/>
-      <c r="T21" s="171"/>
-      <c r="U21" s="172"/>
+      <c r="O21" s="71"/>
+      <c r="P21" s="71"/>
+      <c r="Q21" s="71"/>
+      <c r="R21" s="71"/>
+      <c r="S21" s="71"/>
+      <c r="T21" s="71"/>
+      <c r="U21" s="72"/>
     </row>
     <row r="22" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B22" s="110" t="str">
+      <c r="B22" s="95" t="str">
         <f>IF(AND(B18="Pas de notes", B20="Pas de notes"), "Pas de notes", IF(B18="Pas de notes", B20, IF(B20="Pas de notes", B18, (B18*B5+B20*B12)/(B12+B5))))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="C22" s="111"/>
-      <c r="D22" s="110" t="str">
+      <c r="C22" s="96"/>
+      <c r="D22" s="95" t="str">
         <f>IF(AND(D18="Pas de notes", D20="Pas de notes"), "Pas de notes", IF(D18="Pas de notes", D20, IF(D20="Pas de notes", D18, (D18*D5+D20*D12)/(D12+D5))))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="E22" s="111"/>
-      <c r="F22" s="151" t="str">
+      <c r="E22" s="96"/>
+      <c r="F22" s="43" t="str">
         <f>IF(AND(F18="Pas de notes", F20="Pas de notes"), "Pas de notes", IF(F18="Pas de notes", F20, IF(F20="Pas de notes", F18, (F18*F5+F20*F12)/(F12+F5))))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="G22" s="152"/>
-      <c r="H22" s="151" t="str">
+      <c r="G22" s="44"/>
+      <c r="H22" s="43" t="str">
         <f>IF(AND(H18="Pas de notes", H20="Pas de notes"), "Pas de notes", IF(H18="Pas de notes", H20, IF(H20="Pas de notes", H18, (H18*H5+H20*H12)/(H12+H5))))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="I22" s="152"/>
-      <c r="J22" s="122" t="str">
+      <c r="I22" s="44"/>
+      <c r="J22" s="80" t="str">
         <f>IF(AND(J18="Pas de notes", J20="Pas de notes"), "Pas de notes", IF(J18="Pas de notes", J20, IF(J20="Pas de notes", J18, (J18*J5+J20*J12)/(J12+J5))))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="K22" s="123"/>
-      <c r="L22" s="122" t="str">
+      <c r="K22" s="81"/>
+      <c r="L22" s="80" t="str">
         <f>IF(OR(L18="Pas de notes", L20="Pas de notes"),"Pas de notes",((L18*L5+L20*L12)/(L12+L5)))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="M22" s="123"/>
-      <c r="N22" s="173"/>
-      <c r="O22" s="174"/>
-      <c r="P22" s="174"/>
-      <c r="Q22" s="174"/>
-      <c r="R22" s="174"/>
-      <c r="S22" s="174"/>
-      <c r="T22" s="174"/>
-      <c r="U22" s="175"/>
+      <c r="M22" s="81"/>
+      <c r="N22" s="73"/>
+      <c r="O22" s="74"/>
+      <c r="P22" s="74"/>
+      <c r="Q22" s="74"/>
+      <c r="R22" s="74"/>
+      <c r="S22" s="74"/>
+      <c r="T22" s="74"/>
+      <c r="U22" s="75"/>
     </row>
     <row r="23" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B23" s="112" t="s">
+      <c r="B23" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="113"/>
-      <c r="D23" s="113"/>
-      <c r="E23" s="114"/>
-      <c r="F23" s="153" t="s">
+      <c r="C23" s="98"/>
+      <c r="D23" s="98"/>
+      <c r="E23" s="99"/>
+      <c r="F23" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="154"/>
-      <c r="H23" s="154"/>
-      <c r="I23" s="154"/>
-      <c r="J23" s="159" t="s">
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="K23" s="159"/>
-      <c r="L23" s="159"/>
-      <c r="M23" s="160"/>
-      <c r="N23" s="173"/>
-      <c r="O23" s="174"/>
-      <c r="P23" s="174"/>
-      <c r="Q23" s="174"/>
-      <c r="R23" s="174"/>
-      <c r="S23" s="174"/>
-      <c r="T23" s="174"/>
-      <c r="U23" s="175"/>
+      <c r="K23" s="59"/>
+      <c r="L23" s="59"/>
+      <c r="M23" s="60"/>
+      <c r="N23" s="73"/>
+      <c r="O23" s="74"/>
+      <c r="P23" s="74"/>
+      <c r="Q23" s="74"/>
+      <c r="R23" s="74"/>
+      <c r="S23" s="74"/>
+      <c r="T23" s="74"/>
+      <c r="U23" s="75"/>
     </row>
     <row r="24" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B24" s="115" t="str">
-        <f>IF(AND(B22="Pas de notes", D22="Pas de notes"), "Pas de notes", IF(B22="Pas de notes", D22, IF(D22="Pas de notes", B22, (B22+D22)/2)))</f>
+      <c r="B24" s="100" t="str">
+        <f>IF(AND(B22="Pas de notes", D22="Pas de notes"), "Pas de notes", IF(B22="Pas de notes", D22, IF(D22="Pas de notes", B22, (B22*B3+D22*D3)/(B3+D3))))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="C24" s="116"/>
-      <c r="D24" s="116"/>
-      <c r="E24" s="117"/>
-      <c r="F24" s="155" t="str">
-        <f>IF(AND(F22="Pas de notes", H22="Pas de notes"), "Pas de notes", IF(F22="Pas de notes", H22, IF(H22="Pas de notes", F22, (F22+H22)/2)))</f>
+      <c r="C24" s="101"/>
+      <c r="D24" s="101"/>
+      <c r="E24" s="102"/>
+      <c r="F24" s="47" t="str">
+        <f>IF(AND(F22="Pas de notes",H22="Pas de notes"),"Pas de notes",IF(F22="Pas de notes",H22,IF(H22="Pas de notes",F22,(F22*F3+H22*H3)/(F3+H3))))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="G24" s="156"/>
-      <c r="H24" s="156"/>
-      <c r="I24" s="157"/>
-      <c r="J24" s="161" t="str">
-        <f>IF(AND(J22="Pas de notes", L22="Pas de notes"), "Pas de notes", IF(J22="Pas de notes", L22, IF(L22="Pas de notes", J22, (J22+L22)/2)))</f>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="61" t="str">
+        <f>IF(AND(J22="Pas de notes",L22="Pas de notes"),"Pas de notes",IF(J22="Pas de notes",L22,IF(L22="Pas de notes",J22,(J22*J3+L22*L3)/(J3+L3))))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="K24" s="162"/>
-      <c r="L24" s="162"/>
-      <c r="M24" s="163"/>
-      <c r="N24" s="167" t="str">
-        <f>IF(AND(N20="Pas de notes", R20="Pas de notes"), "Pas de notes", IF(N20="Pas de notes", R20, IF(R20="Pas de notes", N20, (N20+R20)/2)))</f>
+      <c r="K24" s="62"/>
+      <c r="L24" s="62"/>
+      <c r="M24" s="63"/>
+      <c r="N24" s="67" t="str">
+        <f>IF(AND(R18="Pas de notes", T18="Pas de notes"), "Pas de notes", IF(R18="Pas de notes", T18, IF(P18="Pas de notes", N18, (N18+P18)/2)))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="O24" s="168"/>
-      <c r="P24" s="168"/>
-      <c r="Q24" s="168"/>
-      <c r="R24" s="168"/>
-      <c r="S24" s="168"/>
-      <c r="T24" s="168"/>
-      <c r="U24" s="169"/>
+      <c r="O24" s="68"/>
+      <c r="P24" s="68"/>
+      <c r="Q24" s="68"/>
+      <c r="R24" s="68"/>
+      <c r="S24" s="68"/>
+      <c r="T24" s="68"/>
+      <c r="U24" s="69"/>
     </row>
     <row r="25" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B25" s="133" t="s">
+      <c r="B25" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="134"/>
-      <c r="D25" s="134"/>
-      <c r="E25" s="134"/>
-      <c r="F25" s="134"/>
-      <c r="G25" s="134"/>
-      <c r="H25" s="134"/>
-      <c r="I25" s="134"/>
-      <c r="J25" s="134"/>
-      <c r="K25" s="134"/>
-      <c r="L25" s="134"/>
-      <c r="M25" s="134"/>
-      <c r="N25" s="134"/>
-      <c r="O25" s="134"/>
-      <c r="P25" s="134"/>
-      <c r="Q25" s="134"/>
-      <c r="R25" s="134"/>
-      <c r="S25" s="134"/>
-      <c r="T25" s="134"/>
-      <c r="U25" s="135"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="26"/>
+      <c r="P25" s="26"/>
+      <c r="Q25" s="26"/>
+      <c r="R25" s="26"/>
+      <c r="S25" s="26"/>
+      <c r="T25" s="26"/>
+      <c r="U25" s="27"/>
     </row>
     <row r="26" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B26" s="136"/>
-      <c r="C26" s="137"/>
-      <c r="D26" s="137"/>
-      <c r="E26" s="137"/>
-      <c r="F26" s="137"/>
-      <c r="G26" s="137"/>
-      <c r="H26" s="137"/>
-      <c r="I26" s="137"/>
-      <c r="J26" s="137"/>
-      <c r="K26" s="137"/>
-      <c r="L26" s="137"/>
-      <c r="M26" s="137"/>
-      <c r="N26" s="137"/>
-      <c r="O26" s="137"/>
-      <c r="P26" s="137"/>
-      <c r="Q26" s="137"/>
-      <c r="R26" s="137"/>
-      <c r="S26" s="137"/>
-      <c r="T26" s="137"/>
-      <c r="U26" s="138"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="29"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="29"/>
+      <c r="Q26" s="29"/>
+      <c r="R26" s="29"/>
+      <c r="S26" s="29"/>
+      <c r="T26" s="29"/>
+      <c r="U26" s="30"/>
     </row>
     <row r="27" spans="2:21" ht="14.25" customHeight="1">
       <c r="B27" s="10"/>
-      <c r="C27" s="139" t="str">
+      <c r="C27" s="31" t="str">
         <f>IF(AND(B24="Pas de notes", F24="Pas de notes", N24="Pas de notes", J24="Pas de notes"), "Pas de notes", (IF(B24="Pas de notes", 0, B24*(B3+D3)) + IF(F24="Pas de notes", 0, F24*(F3+H3)) + IF(N24="Pas de notes", 0, N24*(N3+P3+R3+T3)) + IF(J24="Pas de notes", 0, J24*(J3+L3))) / (IF(B24="Pas de notes", 0, B3+D3) + IF(F24="Pas de notes", 0, F3+H3) + IF(N24="Pas de notes", 0, N3+P3+R3+T3) + IF(J24="Pas de notes", 0, J3+L3)))</f>
         <v>Pas de notes</v>
       </c>
-      <c r="D27" s="139"/>
-      <c r="E27" s="139"/>
-      <c r="F27" s="139"/>
-      <c r="G27" s="139"/>
-      <c r="H27" s="139"/>
-      <c r="I27" s="139"/>
-      <c r="J27" s="139"/>
-      <c r="K27" s="139"/>
-      <c r="L27" s="139"/>
-      <c r="M27" s="139"/>
-      <c r="N27" s="139"/>
-      <c r="O27" s="139"/>
-      <c r="P27" s="139"/>
-      <c r="Q27" s="139"/>
-      <c r="R27" s="139"/>
-      <c r="S27" s="139"/>
-      <c r="T27" s="139"/>
-      <c r="U27" s="140"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="31"/>
+      <c r="P27" s="31"/>
+      <c r="Q27" s="31"/>
+      <c r="R27" s="31"/>
+      <c r="S27" s="31"/>
+      <c r="T27" s="31"/>
+      <c r="U27" s="32"/>
     </row>
     <row r="28" spans="2:21" ht="14.25" customHeight="1"/>
     <row r="29" spans="2:21" ht="14.25" customHeight="1"/>
@@ -3668,6 +3678,89 @@
     <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="107">
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L19:M19"/>
     <mergeCell ref="B25:U26"/>
     <mergeCell ref="C27:U27"/>
     <mergeCell ref="N4:U5"/>
@@ -3692,91 +3785,12 @@
     <mergeCell ref="R20:U20"/>
     <mergeCell ref="N21:U23"/>
     <mergeCell ref="N24:U24"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
+  <ignoredErrors>
+    <ignoredError sqref="L18" formulaRange="1"/>
+    <ignoredError sqref="P18" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>